<commit_message>
Execl file updated Post01 Final
</commit_message>
<xml_diff>
--- a/Log of all Blogs.xlsx
+++ b/Log of all Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>S.No</t>
   </si>
@@ -24,44 +24,42 @@
     <t>Date of Post</t>
   </si>
   <si>
-    <t>Link of the Blog Post</t>
-  </si>
-  <si>
     <t>Learn Front-end development :- A Practile Guide to Become Front-end Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">Master CSS :- Top CSS frameworks and resources </t>
-  </si>
-  <si>
     <t>Title of the Blog Post</t>
   </si>
   <si>
-    <t>programmingport/learn.com</t>
-  </si>
-  <si>
-    <t>programmingport/master.com</t>
-  </si>
-  <si>
-    <t>Java Concepts :- Basics of Java Part-01</t>
-  </si>
-  <si>
-    <t>programmingport/java-1</t>
-  </si>
-  <si>
-    <t>Java Concepts :- Basics of Java Part-02</t>
+    <t>Link of the Blog Post on Hashnode</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/learn-front-end-development-a-practical-guide-to-become-front-end-developer</t>
+  </si>
+  <si>
+    <t>Link of the Blog Post on Dev.to</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/learn-front-end-development-a-practical-guide-to-become-front-end-developer-1jfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,16 +79,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -226,17 +228,17 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
             <a:t>Link</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" baseline="0"/>
-            <a:t> of the website :- programmigport.com</a:t>
+            <a:t> of the website :- https://programmingport.hashnode.dev/    https://dev.to/rahulmishra05</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
@@ -248,13 +250,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:E14" totalsRowShown="0">
-  <autoFilter ref="B10:E14"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F11" totalsRowShown="0">
+  <autoFilter ref="B10:F11">
+    <filterColumn colId="4"/>
+  </autoFilter>
+  <tableColumns count="5">
     <tableColumn id="1" name="S.No"/>
     <tableColumn id="2" name="Title of the Blog Post"/>
     <tableColumn id="3" name="Date of Post" dataDxfId="0"/>
-    <tableColumn id="4" name="Link of the Blog Post"/>
+    <tableColumn id="4" name="Link of the Blog Post on Hashnode" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="Link of the Blog Post on Dev.to" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -545,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:E14"/>
+  <dimension ref="B10:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -556,81 +561,54 @@
     <col min="2" max="2" width="10.26953125" customWidth="1"/>
     <col min="3" max="3" width="69.81640625" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="52.36328125" customWidth="1"/>
+    <col min="5" max="5" width="116" customWidth="1"/>
+    <col min="6" max="6" width="133.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:6">
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:6">
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>40940</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1">
-        <v>38048</v>
-      </c>
-      <c r="E12" t="s">
+        <v>44112</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="2">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="3">
-        <v>12480</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="2">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1"/>
+    <hyperlink ref="F11" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Excel file updated after additions of Post02
</commit_message>
<xml_diff>
--- a/Log of all Blogs.xlsx
+++ b/Log of all Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S.No</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/learn-front-end-development-a-practical-guide-to-become-front-end-developer-1jfo</t>
+  </si>
+  <si>
+    <t>Master CSS :- Top CSS Frameworks and Resources</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/master-css-top-css-frameworks-and-resources</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/master-css-top-css-frameworks-and-resources-5gj9</t>
   </si>
 </sst>
 </file>
@@ -86,10 +95,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -250,8 +262,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F11" totalsRowShown="0">
-  <autoFilter ref="B10:F11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F12" totalsRowShown="0">
+  <autoFilter ref="B10:F12">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -550,9 +562,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F11"/>
+  <dimension ref="B10:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -599,16 +611,35 @@
         <v>7</v>
       </c>
     </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
+        <v>44113</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E11" r:id="rId1"/>
     <hyperlink ref="F11" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="F12" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <drawing r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>